<commit_message>
Updated ingredient list to inlclude grains, spices, herbs, cheese, nuts, and onions
</commit_message>
<xml_diff>
--- a/Ingredients.xlsx
+++ b/Ingredients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmaneil/cs334/CS334-Final-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmaneil/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B820BBC7-05B1-CD4F-B33E-CC3CDE285264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7FE7E9-7C91-4342-8311-ED72305EB928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21600" xr2:uid="{13EE0B30-CE7D-4545-9524-AD5F66A30520}"/>
+    <workbookView xWindow="140" yWindow="480" windowWidth="28660" windowHeight="16120" xr2:uid="{13EE0B30-CE7D-4545-9524-AD5F66A30520}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Head</t>
   </si>
   <si>
-    <t>Fava Beans</t>
-  </si>
-  <si>
     <t>Ounce</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Escarole Lettuce</t>
   </si>
   <si>
-    <t>English Pea</t>
-  </si>
-  <si>
     <t>Tomato</t>
   </si>
   <si>
@@ -226,6 +220,156 @@
   </si>
   <si>
     <t>Delicata Squash</t>
+  </si>
+  <si>
+    <t>Nut</t>
+  </si>
+  <si>
+    <t>English Peas</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Red Onion</t>
+  </si>
+  <si>
+    <t>White Onion</t>
+  </si>
+  <si>
+    <t>Sweet Onion</t>
+  </si>
+  <si>
+    <t>Scallions</t>
+  </si>
+  <si>
+    <t>Shallots</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>Farro</t>
+  </si>
+  <si>
+    <t>Freekeh</t>
+  </si>
+  <si>
+    <t>Polenta</t>
+  </si>
+  <si>
+    <t>Quinoa</t>
+  </si>
+  <si>
+    <t>Legume</t>
+  </si>
+  <si>
+    <t>Chickpeas</t>
+  </si>
+  <si>
+    <t>Fresh Fava Beans</t>
+  </si>
+  <si>
+    <t>Dried Fava Beans</t>
+  </si>
+  <si>
+    <t>Black Turtle Beans</t>
+  </si>
+  <si>
+    <t>Borlotti Beans</t>
+  </si>
+  <si>
+    <t>Barley</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>Mozzarella</t>
+  </si>
+  <si>
+    <t>Parmigiano-Reggiano</t>
+  </si>
+  <si>
+    <t>Aged Pecorino Romano</t>
+  </si>
+  <si>
+    <t>Aged Cheddar</t>
+  </si>
+  <si>
+    <t>Spicy Provolone</t>
+  </si>
+  <si>
+    <t>Ricotta</t>
+  </si>
+  <si>
+    <t>Burrata</t>
+  </si>
+  <si>
+    <t>Roasted Walnuts</t>
+  </si>
+  <si>
+    <t>Roasted Pine Nuts</t>
+  </si>
+  <si>
+    <t>Roasted Pecans</t>
+  </si>
+  <si>
+    <t>Roasted Almonds</t>
+  </si>
+  <si>
+    <t>Roasted Hazelnuts</t>
+  </si>
+  <si>
+    <t>Roasted Peanuts</t>
+  </si>
+  <si>
+    <t>Roasted Pistachios</t>
+  </si>
+  <si>
+    <t>Gruyere</t>
+  </si>
+  <si>
+    <t>Herb</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Clove</t>
+  </si>
+  <si>
+    <t>Fresh Rosemary</t>
+  </si>
+  <si>
+    <t>Fresh Thyme</t>
+  </si>
+  <si>
+    <t>Fresh Mint</t>
+  </si>
+  <si>
+    <t>Fresh Parsley</t>
+  </si>
+  <si>
+    <t>Fresh Oregano</t>
+  </si>
+  <si>
+    <t>Tablespoon</t>
+  </si>
+  <si>
+    <t>Fresh Sage</t>
+  </si>
+  <si>
+    <t>Spice</t>
+  </si>
+  <si>
+    <t>Cumin</t>
+  </si>
+  <si>
+    <t>Coriander</t>
+  </si>
+  <si>
+    <t>Curry Powder</t>
   </si>
 </sst>
 </file>
@@ -233,7 +377,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -267,7 +411,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,11 +726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47774A71-CCE7-294D-B3EE-1EEB254815B1}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,7 +768,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2">
         <v>0.25</v>
@@ -650,7 +794,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2">
         <v>0.25</v>
@@ -754,7 +898,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2">
         <v>0.125</v>
@@ -780,7 +924,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2">
         <v>0.125</v>
@@ -838,7 +982,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -864,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -936,14 +1080,14 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
       <c r="D14">
         <v>0</v>
       </c>
@@ -951,10 +1095,10 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -962,13 +1106,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -988,13 +1132,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1003,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -1014,16 +1158,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1032,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -1040,16 +1184,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1058,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -1066,13 +1210,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1092,13 +1236,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1107,10 +1251,10 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="s">
         <v>32</v>
@@ -1118,13 +1262,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1144,13 +1288,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1170,13 +1314,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1196,13 +1340,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1222,22 +1366,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1254,7 +1398,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1274,22 +1418,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1300,22 +1444,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B28" s="2">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1326,13 +1470,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B29" s="2">
-        <v>0.125</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1352,22 +1496,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1378,19 +1522,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1404,13 +1548,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1419,10 +1563,10 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="s">
         <v>32</v>
@@ -1430,25 +1574,25 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
         <v>32</v>
@@ -1456,25 +1600,25 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
         <v>32</v>
@@ -1482,13 +1626,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1508,25 +1652,25 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="s">
         <v>32</v>
@@ -1540,13 +1684,13 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1560,19 +1704,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1586,22 +1730,22 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B39" s="2">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -1612,13 +1756,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B40" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1638,22 +1782,22 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B41" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41">
-        <v>0</v>
+      <c r="F41" s="1">
+        <v>1</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1664,13 +1808,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B42" s="2">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1682,21 +1826,21 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B43" s="2">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1704,25 +1848,25 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="B44" s="2">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1730,25 +1874,25 @@
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="B45" s="2">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1756,25 +1900,25 @@
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="B46" s="2">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1782,25 +1926,25 @@
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="B47" s="2">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1808,40 +1952,1106 @@
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>1</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="C57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="C58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="C59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="C60" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B62" s="2">
         <v>0.125</v>
       </c>
-      <c r="C48" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
+      <c r="C62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" s="2">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="2">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="2">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="2">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="2">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>106</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>106</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>106</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C85" t="s">
+        <v>106</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>107</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>106</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>106</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>110</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C89" t="s">
+        <v>106</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>